<commit_message>
added combined income csv and combined income/gdp csv
</commit_message>
<xml_diff>
--- a/GDP 1969-2020/GDP_1969_2020.xlsx
+++ b/GDP 1969-2020/GDP_1969_2020.xlsx
@@ -377,7 +377,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -620,190 +620,198 @@
         <v>1997</v>
       </c>
       <c r="B30">
-        <v>8577552</v>
+        <v>8284431.7</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B31">
-        <v>9062817</v>
+        <v>8577552</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B32">
-        <v>9630663</v>
+        <v>9062817</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B33">
-        <v>10252347</v>
+        <v>9630663</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B34">
-        <v>10581822</v>
+        <v>10252347</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B35">
-        <v>10936418</v>
+        <v>10581822</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B36">
-        <v>11458246</v>
+        <v>10936418</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B37">
-        <v>12213730</v>
+        <v>11458246</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B38">
-        <v>13036637</v>
+        <v>12213730</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B39">
-        <v>13814609</v>
+        <v>13036637</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B40">
-        <v>14451860</v>
+        <v>13814609</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B41">
-        <v>14712845</v>
+        <v>14451860</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B42">
-        <v>14448932</v>
+        <v>14712845</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B43">
-        <v>14992052</v>
+        <v>14448932</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B44">
-        <v>15542582</v>
+        <v>14992052</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B45">
-        <v>16197007</v>
+        <v>15542582</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B46">
-        <v>16784851</v>
+        <v>16197007</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B47">
-        <v>17527258</v>
+        <v>16784851</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B48">
-        <v>18238301</v>
+        <v>17527258</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B49">
-        <v>18745075</v>
+        <v>18238301</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B50">
-        <v>19542980</v>
+        <v>18745075</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B51">
-        <v>20611861</v>
+        <v>19542980</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B52">
-        <v>21433226</v>
+        <v>20611861</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53">
+        <v>2019</v>
+      </c>
+      <c r="B53">
+        <v>21433226</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
         <v>2020</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>20936558</v>
       </c>
     </row>

</xml_diff>